<commit_message>
fix(import names for mautic)
</commit_message>
<xml_diff>
--- a/merged_profiles_mautic.xlsx
+++ b/merged_profiles_mautic.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>first_name</t>
+          <t>First Name</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>last_name</t>
+          <t>Last Name</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -456,12 +456,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>location</t>
+          <t>Address Line 1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>linked_in</t>
+          <t>LinkedIn</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>industry</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">

</xml_diff>

<commit_message>
fix(company name is a required field in mautic)
</commit_message>
<xml_diff>
--- a/merged_profiles_mautic.xlsx
+++ b/merged_profiles_mautic.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>First Name</t>
+          <t>firstname</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Last Name</t>
+          <t>lastname</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -456,12 +456,12 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Address Line 1</t>
+          <t>address1</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>LinkedIn</t>
+          <t>linkedin</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -496,7 +496,7 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Industry</t>
+          <t>companyindustry</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">

</xml_diff>